<commit_message>
2012-02-17 Complete sync of papers, posters and spreadsheets
</commit_message>
<xml_diff>
--- a/media/spreadsheets/DCast-vs-Visitors.xlsx
+++ b/media/spreadsheets/DCast-vs-Visitors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
     <sheet name="Sheet8" sheetId="8" r:id="rId7"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId8"/>
+    <sheet name="Performance" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="synthetic_dynamic_cast_gcd1" localSheetId="0">Sheet1!$A$1:$W$100</definedName>
@@ -24,7 +25,7 @@
     <definedName name="synthetic_select_random_memoized_mat" localSheetId="6">Sheet8!$A$1:$W$100</definedName>
     <definedName name="synthetic_select_random_vis" localSheetId="4">Sheet4!$A$1:$W$100</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -208,7 +209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8411" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8449" uniqueCount="33">
   <si>
     <t>AreaVisSeq</t>
   </si>
@@ -269,6 +270,45 @@
   <si>
     <t>Exception</t>
   </si>
+  <si>
+    <t>4.6.1</t>
+  </si>
+  <si>
+    <t>4.6.1 FP</t>
+  </si>
+  <si>
+    <t>4.5.2</t>
+  </si>
+  <si>
+    <t>VC++2010</t>
+  </si>
+  <si>
+    <t>Mat</t>
+  </si>
+  <si>
+    <t>Seq</t>
+  </si>
+  <si>
+    <t>Rnd</t>
+  </si>
+  <si>
+    <t>Rep</t>
+  </si>
+  <si>
+    <t>NO PGO</t>
+  </si>
+  <si>
+    <t>VC++ PGO</t>
+  </si>
+  <si>
+    <t>VC++</t>
+  </si>
+  <si>
+    <t>Visitors</t>
+  </si>
+  <si>
+    <t>Type Switch</t>
+  </si>
 </sst>
 </file>
 
@@ -291,7 +331,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -299,12 +339,129 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1866,11 +2023,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="145209600"/>
-        <c:axId val="143720832"/>
+        <c:axId val="149541248"/>
+        <c:axId val="149543168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="145209600"/>
+        <c:axId val="149541248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1905,7 +2062,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143720832"/>
+        <c:crossAx val="149543168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1913,7 +2070,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143720832"/>
+        <c:axId val="149543168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1950,7 +2107,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145209600"/>
+        <c:crossAx val="149541248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3478,11 +3635,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="143761792"/>
-        <c:axId val="143763712"/>
+        <c:axId val="148809984"/>
+        <c:axId val="148861312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="143761792"/>
+        <c:axId val="148809984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3527,7 +3684,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="143763712"/>
+        <c:crossAx val="148861312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3536,7 +3693,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143763712"/>
+        <c:axId val="148861312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3559,14 +3716,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143761792"/>
+        <c:crossAx val="148809984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4607,11 +4763,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="148678144"/>
-        <c:axId val="148679680"/>
+        <c:axId val="149613952"/>
+        <c:axId val="149755008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="148678144"/>
+        <c:axId val="149613952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4620,7 +4776,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148679680"/>
+        <c:crossAx val="149755008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4628,7 +4784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148679680"/>
+        <c:axId val="149755008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4639,7 +4795,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148678144"/>
+        <c:crossAx val="149613952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4654,6 +4810,1376 @@
           <c:y val="0.62461614173228341"/>
           <c:w val="0.26101443569553806"/>
           <c:h val="0.25115157480314959"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="30"/>
+      <c:rAngAx val="0"/>
+      <c:perspective val="20"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.6.1 FP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Performance!$B$1:$G$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Vis</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Mat</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Vis</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Mat</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Vis</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Mat</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Rnd</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Seq</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Rep</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Performance!$B$3:$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.6.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Performance!$B$1:$G$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Vis</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Mat</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Vis</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Mat</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Vis</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Mat</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Rnd</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Seq</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Rep</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Performance!$B$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.5.2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Performance!$B$1:$G$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Vis</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Mat</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Vis</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Mat</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Vis</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Mat</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Rnd</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Seq</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Rep</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Performance!$B$5:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>VC++2010</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Performance!$B$1:$G$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Vis</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Mat</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Vis</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Mat</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Vis</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Mat</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Rnd</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Seq</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Rep</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Performance!$B$6:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NO PGO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Performance!$B$1:$G$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Vis</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Mat</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Vis</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Mat</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Vis</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Mat</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Rnd</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Seq</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Rep</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Performance!$B$7:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="150182144"/>
+        <c:axId val="150188032"/>
+        <c:axId val="150184384"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="150182144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="150188032"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="150188032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="150182144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="150184384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="150188032"/>
+        <c:crosses val="autoZero"/>
+      </c:serAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Random</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.22029883136116366"/>
+          <c:y val="4.5176589503007139E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10866178334465189"/>
+          <c:y val="5.3538381159009774E-2"/>
+          <c:w val="0.86241587120045748"/>
+          <c:h val="0.80314541425072639"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Visitors</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Performance!$A$10:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.6.1 FP</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>VC++ PGO</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>VC++</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Performance!$B$10:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Type Switch</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Performance!$A$10:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.6.1 FP</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>VC++ PGO</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>VC++</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Performance!$C$10:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="149829504"/>
+        <c:axId val="149831040"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="149829504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="149831040"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="149831040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="60"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Cycles/iteration</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="8.771929824561403E-2"/>
+              <c:y val="0.27450166750604971"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="149829504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.677985564304462"/>
+          <c:y val="2.2203856453217707E-2"/>
+          <c:w val="0.28973649675369528"/>
+          <c:h val="0.11170985494721798"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Sequential</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.22319108472096727"/>
+          <c:y val="4.3010752688172046E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10567105717289926"/>
+          <c:y val="5.2032907948818055E-2"/>
+          <c:w val="0.86743152783135535"/>
+          <c:h val="0.82867171015387786"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Visitors</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Performance!$A$17:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.6.1 FP</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>VC++ PGO</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>VC++</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Performance!$B$17:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$C$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Type Switch</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Performance!$A$17:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.6.1 FP</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>VC++ PGO</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>VC++</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Performance!$C$17:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="149850368"/>
+        <c:axId val="149864448"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="149850368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="149864448"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="149864448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="60"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Cycles/iteration</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="8.7431693989071038E-2"/>
+              <c:y val="0.2988773177546355"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="149850368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.67748238027623597"/>
+          <c:y val="2.6081524755642103E-2"/>
+          <c:w val="0.27282578202314872"/>
+          <c:h val="0.10736770806874947"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Repetitive</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.20162317945550923"/>
+          <c:y val="4.744956708808358E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10664949288746314"/>
+          <c:y val="5.1941612561587698E-2"/>
+          <c:w val="0.86700079624878346"/>
+          <c:h val="0.83850451295468942"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$B$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Visitors</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Performance!$A$24:$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.6.1 FP</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>VC++ PGO</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>VC++</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Performance!$B$24:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$C$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Type Switch</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Performance!$A$24:$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.6.1 FP</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>VC++ PGO</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>VC++</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Performance!$C$24:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="150208512"/>
+        <c:axId val="150210048"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="150208512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="150210048"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="150210048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="60"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Cycles/iteration</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="8.2788671023965144E-2"/>
+              <c:y val="0.29540493908895338"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="150208512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.67841524711371859"/>
+          <c:y val="2.6631162932846533E-2"/>
+          <c:w val="0.26929717118693497"/>
+          <c:h val="0.10369977437030897"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4762,6 +6288,131 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>485776</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -26497,7 +28148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
@@ -51805,4 +53456,385 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1">
+        <v>60</v>
+      </c>
+      <c r="C3" s="3">
+        <v>53</v>
+      </c>
+      <c r="D3" s="1">
+        <v>58</v>
+      </c>
+      <c r="E3" s="3">
+        <v>55</v>
+      </c>
+      <c r="F3" s="2">
+        <v>28</v>
+      </c>
+      <c r="G3" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4">
+        <v>47</v>
+      </c>
+      <c r="C4" s="6">
+        <v>53</v>
+      </c>
+      <c r="D4" s="4">
+        <v>48</v>
+      </c>
+      <c r="E4" s="6">
+        <v>53</v>
+      </c>
+      <c r="F4" s="5">
+        <v>18</v>
+      </c>
+      <c r="G4" s="6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="4">
+        <v>56</v>
+      </c>
+      <c r="C5" s="6">
+        <v>55</v>
+      </c>
+      <c r="D5" s="4">
+        <v>55</v>
+      </c>
+      <c r="E5" s="6">
+        <v>49</v>
+      </c>
+      <c r="F5" s="5">
+        <v>26</v>
+      </c>
+      <c r="G5" s="6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4">
+        <v>48</v>
+      </c>
+      <c r="C6" s="6">
+        <v>54</v>
+      </c>
+      <c r="D6" s="4">
+        <v>45</v>
+      </c>
+      <c r="E6" s="6">
+        <v>31</v>
+      </c>
+      <c r="F6" s="5">
+        <v>19</v>
+      </c>
+      <c r="G6" s="6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="7">
+        <v>49</v>
+      </c>
+      <c r="C7" s="9">
+        <v>51</v>
+      </c>
+      <c r="D7" s="7">
+        <v>49</v>
+      </c>
+      <c r="E7" s="9">
+        <v>52</v>
+      </c>
+      <c r="F7" s="8">
+        <v>18</v>
+      </c>
+      <c r="G7" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1">
+        <v>60</v>
+      </c>
+      <c r="C10" s="3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="4">
+        <v>47</v>
+      </c>
+      <c r="C11" s="6">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="4">
+        <v>56</v>
+      </c>
+      <c r="C12" s="6">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="4">
+        <v>48</v>
+      </c>
+      <c r="C13" s="6">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="7">
+        <v>49</v>
+      </c>
+      <c r="C14" s="9">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="1">
+        <v>58</v>
+      </c>
+      <c r="C17" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="4">
+        <v>48</v>
+      </c>
+      <c r="C18" s="6">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="4">
+        <v>55</v>
+      </c>
+      <c r="C19" s="6">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="4">
+        <v>45</v>
+      </c>
+      <c r="C20" s="6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="7">
+        <v>49</v>
+      </c>
+      <c r="C21" s="9">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1">
+        <v>28</v>
+      </c>
+      <c r="C24" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="4">
+        <v>18</v>
+      </c>
+      <c r="C25" s="6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="4">
+        <v>26</v>
+      </c>
+      <c r="C26" s="6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="4">
+        <v>19</v>
+      </c>
+      <c r="C27" s="6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="7">
+        <v>18</v>
+      </c>
+      <c r="C28" s="9">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated media files for OOPSLA 2012 camera-ready submission
</commit_message>
<xml_diff>
--- a/media/spreadsheets/DCast-vs-Visitors.xlsx
+++ b/media/spreadsheets/DCast-vs-Visitors.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="1" activeTab="9"/>
@@ -2045,11 +2045,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="140837632"/>
-        <c:axId val="140839552"/>
+        <c:axId val="79765504"/>
+        <c:axId val="79901056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140837632"/>
+        <c:axId val="79765504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2084,7 +2084,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140839552"/>
+        <c:crossAx val="79901056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2092,7 +2092,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140839552"/>
+        <c:axId val="79901056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2129,7 +2129,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140837632"/>
+        <c:crossAx val="79765504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3657,11 +3657,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="140872320"/>
-        <c:axId val="140874496"/>
+        <c:axId val="91521792"/>
+        <c:axId val="91524096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140872320"/>
+        <c:axId val="91521792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3706,7 +3706,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140874496"/>
+        <c:crossAx val="91524096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3715,7 +3715,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140874496"/>
+        <c:axId val="91524096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3745,7 +3745,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140872320"/>
+        <c:crossAx val="91521792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4786,11 +4786,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="141582336"/>
-        <c:axId val="141583872"/>
+        <c:axId val="147908480"/>
+        <c:axId val="147931136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="141582336"/>
+        <c:axId val="147908480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4799,7 +4799,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141583872"/>
+        <c:crossAx val="147931136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4807,7 +4807,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141583872"/>
+        <c:axId val="147931136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4818,7 +4818,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141582336"/>
+        <c:crossAx val="147908480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5305,12 +5305,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="142199424"/>
-        <c:axId val="142209408"/>
-        <c:axId val="142205824"/>
+        <c:axId val="152078592"/>
+        <c:axId val="153530368"/>
+        <c:axId val="94663104"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="142199424"/>
+        <c:axId val="152078592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5319,7 +5319,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142209408"/>
+        <c:crossAx val="153530368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5327,7 +5327,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142209408"/>
+        <c:axId val="153530368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5338,12 +5338,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142199424"/>
+        <c:crossAx val="152078592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="142205824"/>
+        <c:axId val="94663104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5352,7 +5352,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142209408"/>
+        <c:crossAx val="153530368"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -5565,11 +5565,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="141641984"/>
-        <c:axId val="141643776"/>
+        <c:axId val="237561344"/>
+        <c:axId val="237562880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="141641984"/>
+        <c:axId val="237561344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5578,7 +5578,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141643776"/>
+        <c:crossAx val="237562880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5586,7 +5586,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141643776"/>
+        <c:axId val="237562880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -5624,7 +5624,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141641984"/>
+        <c:crossAx val="237561344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5847,11 +5847,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="141681792"/>
-        <c:axId val="141683328"/>
+        <c:axId val="265073792"/>
+        <c:axId val="39661568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="141681792"/>
+        <c:axId val="265073792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5860,7 +5860,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141683328"/>
+        <c:crossAx val="39661568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5868,7 +5868,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141683328"/>
+        <c:axId val="39661568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -5906,7 +5906,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141681792"/>
+        <c:crossAx val="265073792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6129,11 +6129,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="141843840"/>
-        <c:axId val="142238848"/>
+        <c:axId val="39670528"/>
+        <c:axId val="39672064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="141843840"/>
+        <c:axId val="39670528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6142,7 +6142,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142238848"/>
+        <c:crossAx val="39672064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6150,7 +6150,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142238848"/>
+        <c:axId val="39672064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -6188,7 +6188,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141843840"/>
+        <c:crossAx val="39670528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6264,7 +6264,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="15875">
+            <a:ln w="12700">
               <a:prstDash val="lgDash"/>
             </a:ln>
           </c:spPr>
@@ -6906,8 +6906,8 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="15875">
-              <a:prstDash val="dash"/>
+            <a:ln w="12700">
+              <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -7548,7 +7548,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="15875">
+            <a:ln w="12700">
               <a:prstDash val="sysDash"/>
             </a:ln>
           </c:spPr>
@@ -8190,8 +8190,8 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="15875">
-              <a:prstDash val="solid"/>
+            <a:ln w="25400">
+              <a:prstDash val="sysDot"/>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -8832,8 +8832,13 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050">
-              <a:prstDash val="sysDot"/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="lgDashDot"/>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -9469,11 +9474,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="142365824"/>
-        <c:axId val="142367360"/>
+        <c:axId val="39684352"/>
+        <c:axId val="39686528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="142365824"/>
+        <c:axId val="39684352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9486,10 +9491,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1000"/>
                   <a:t>Case</a:t>
                 </a:r>
               </a:p>
@@ -9499,8 +9504,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.0244893301380807E-3"/>
-              <c:y val="0.94123656282095169"/>
+              <c:x val="1.0244973607395258E-3"/>
+              <c:y val="0.91815636681778412"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -9509,7 +9514,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142367360"/>
+        <c:crossAx val="39686528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9519,7 +9524,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142367360"/>
+        <c:axId val="39686528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="140"/>
@@ -9547,8 +9552,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="6.9979806303281863E-2"/>
-              <c:y val="0.41682852143482063"/>
+              <c:x val="7.320208705182997E-2"/>
+              <c:y val="0.38652549113179036"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -9557,7 +9562,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142365824"/>
+        <c:crossAx val="39684352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12836,11 +12841,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="143433728"/>
-        <c:axId val="89741952"/>
+        <c:axId val="39701888"/>
+        <c:axId val="39707776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="143433728"/>
+        <c:axId val="39701888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12850,7 +12855,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89741952"/>
+        <c:crossAx val="39707776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12860,7 +12865,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89741952"/>
+        <c:axId val="39707776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="140"/>
@@ -12872,7 +12877,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143433728"/>
+        <c:crossAx val="39701888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20646,8 +20651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64096,7 +64101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B23" sqref="B23:C23"/>
     </sheetView>
   </sheetViews>

</xml_diff>